<commit_message>
REALIZANDO EJERCICIOS DE NIVEL AVANZADO DE EXCEL
</commit_message>
<xml_diff>
--- a/Nivel Avanzado/Modulo9/BI primeros ejercicios.xlsx
+++ b/Nivel Avanzado/Modulo9/BI primeros ejercicios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AllisonGuizado\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\db\Nik Denilson\Cursos\EXCEL\Nivel Avanzado\Modulo9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BF63FD4-54C4-4608-B79B-2F4FED5DDA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A79C60-8F5E-45BA-B61A-B40B34A57A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33735" yWindow="975" windowWidth="11985" windowHeight="13740" xr2:uid="{97695EB7-5D60-4356-9820-794710C8B368}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{97695EB7-5D60-4356-9820-794710C8B368}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,7 +246,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -259,8 +287,25 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E1D7FD6-77E4-4C0D-B4E3-604D62F01078}" name="Tabla1" displayName="Tabla1" ref="C1:J25" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="C1:J25" xr:uid="{2E1D7FD6-77E4-4C0D-B4E3-604D62F01078}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{166E76F0-E905-4349-A95F-A391F05BEF5A}" name="Proveedor"/>
+    <tableColumn id="2" xr3:uid="{8BF1681B-211B-457A-AF29-61C6A3289025}" name="Categoría"/>
+    <tableColumn id="3" xr3:uid="{8143AE1E-0E4B-4DB7-9AD8-57C280AB4FBB}" name="CantidadPorUnidad"/>
+    <tableColumn id="4" xr3:uid="{59346715-2CBB-49DD-9CAC-31F6F6B67C47}" name="PrecioUnidad " dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2AC6ED12-438F-48B8-B5E1-0F0BBDBB7CCC}" name="UnidadesEnExistencia"/>
+    <tableColumn id="6" xr3:uid="{1F284AF7-644C-4D2C-A048-81E6EBCD9E01}" name="UnidadesEnPedido"/>
+    <tableColumn id="7" xr3:uid="{4C7432B3-E05D-429B-887F-C46E2D81E1FA}" name="NivelNuevoPedido"/>
+    <tableColumn id="8" xr3:uid="{2B31B139-B674-4563-9BC5-3DF2A16E3295}" name="Suspendido"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -559,24 +604,24 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10">
+    <row r="1" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="3:10">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>8</v>
       </c>
@@ -628,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:10">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -654,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:10">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>8</v>
       </c>
@@ -680,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:10">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>14</v>
       </c>
@@ -706,7 +751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:10">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -732,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:10">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>17</v>
       </c>
@@ -758,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:10">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -784,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:10">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>17</v>
       </c>
@@ -810,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:10">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>22</v>
       </c>
@@ -836,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:10">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>22</v>
       </c>
@@ -862,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="3:10">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>27</v>
       </c>
@@ -888,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:10">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -914,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:10">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>31</v>
       </c>
@@ -940,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:10">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>31</v>
       </c>
@@ -966,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:10">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>31</v>
       </c>
@@ -992,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:10">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>35</v>
       </c>
@@ -1018,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:10">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>35</v>
       </c>
@@ -1044,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:10">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>35</v>
       </c>
@@ -1070,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>40</v>
       </c>
@@ -1096,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:10">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>40</v>
       </c>
@@ -1122,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:10">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>40</v>
       </c>
@@ -1148,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:10">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>44</v>
       </c>
@@ -1174,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:10">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>44</v>
       </c>
@@ -1200,7 +1245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:10">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>48</v>
       </c>
@@ -1229,5 +1274,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>